<commit_message>
Added some additional functions to alt-mode
</commit_message>
<xml_diff>
--- a/ui mockup.xlsx
+++ b/ui mockup.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
   <si>
     <t>.</t>
   </si>
@@ -65,9 +65,6 @@
     <t>abs</t>
   </si>
   <si>
-    <t>&lt;-</t>
-  </si>
-  <si>
     <t>sqrt</t>
   </si>
   <si>
@@ -81,13 +78,31 @@
   </si>
   <si>
     <t>1.25 x * x cos *</t>
+  </si>
+  <si>
+    <t>def. view</t>
+  </si>
+  <si>
+    <t>asin</t>
+  </si>
+  <si>
+    <t>acos</t>
+  </si>
+  <si>
+    <t>atan</t>
+  </si>
+  <si>
+    <t>log</t>
+  </si>
+  <si>
+    <t>«</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,6 +116,24 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="FreeSans"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="0"/>
+      <name val="FreeSans"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -167,29 +200,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -479,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="48" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -490,9 +523,9 @@
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="48" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="48" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -500,104 +533,199 @@
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
       <c r="G1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="48" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3">
+        <v>9</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="3">
+        <v>7</v>
+      </c>
+      <c r="J2" s="3">
+        <v>8</v>
+      </c>
+      <c r="K2" s="3">
+        <v>9</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="48" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3">
+        <v>6</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>13</v>
       </c>
+      <c r="F3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="3">
+        <v>4</v>
+      </c>
+      <c r="J3" s="3">
+        <v>5</v>
+      </c>
+      <c r="K3" s="3">
+        <v>6</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" ht="48" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
-        <v>7</v>
-      </c>
-      <c r="B2" s="4">
+    <row r="4" spans="1:15" ht="48" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3">
+        <v>3</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="4">
-        <v>9</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>12</v>
+      <c r="I4" s="3">
+        <v>1</v>
+      </c>
+      <c r="J4" s="3">
+        <v>2</v>
+      </c>
+      <c r="K4" s="3">
+        <v>3</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="48" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
+    <row r="5" spans="1:15" ht="48" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>0</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4">
-        <v>5</v>
-      </c>
-      <c r="C3" s="4">
-        <v>6</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="8" t="s">
+      <c r="E5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="G5" s="8"/>
+      <c r="I5" s="3">
+        <v>0</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="N5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="O5" s="8"/>
     </row>
-    <row r="4" spans="1:7" ht="48" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
-        <v>1</v>
-      </c>
-      <c r="B4" s="4">
-        <v>2</v>
-      </c>
-      <c r="C4" s="4">
-        <v>3</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="48" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
-        <v>0</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:7" ht="48" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:15" ht="48" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="F5:G5"/>
+    <mergeCell ref="I1:N1"/>
+    <mergeCell ref="N5:O5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>